<commit_message>
docs(audit): ajout du retour sur l'existant
</commit_message>
<xml_diff>
--- a/docs/audit/srs-plan.xlsx
+++ b/docs/audit/srs-plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Formations\Aston\ALG\audit\docs\audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFED8BA-8EBB-464E-A0B9-594FB405EBA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F1669A-1A64-40C5-A218-8792EAC2CC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>Legal</t>
+  </si>
+  <si>
+    <t>A faire</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -517,7 +523,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,6 +533,7 @@
     <col min="4" max="4" width="3.44140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="64.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.6640625" customWidth="1"/>
+    <col min="7" max="7" width="27.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -568,6 +575,9 @@
       <c r="F2" t="s">
         <v>28</v>
       </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="str">
@@ -589,6 +599,9 @@
       <c r="F3" t="s">
         <v>29</v>
       </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="str">
@@ -610,6 +623,9 @@
       <c r="F4" t="s">
         <v>30</v>
       </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="str">
@@ -631,6 +647,9 @@
       <c r="F5" t="s">
         <v>29</v>
       </c>
+      <c r="G5" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="str">
@@ -652,6 +671,9 @@
       <c r="F6" t="s">
         <v>28</v>
       </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="str">
@@ -673,6 +695,9 @@
       <c r="F7" t="s">
         <v>29</v>
       </c>
+      <c r="G7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="str">
@@ -694,6 +719,9 @@
       <c r="F8" t="s">
         <v>30</v>
       </c>
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="str">
@@ -715,6 +743,9 @@
       <c r="F9" t="s">
         <v>29</v>
       </c>
+      <c r="G9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="str">
@@ -736,6 +767,9 @@
       <c r="F10" t="s">
         <v>28</v>
       </c>
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="str">
@@ -757,6 +791,9 @@
       <c r="F11" t="s">
         <v>29</v>
       </c>
+      <c r="G11" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="str">
@@ -778,6 +815,9 @@
       <c r="F12" t="s">
         <v>30</v>
       </c>
+      <c r="G12" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="str">
@@ -799,6 +839,9 @@
       <c r="F13" t="s">
         <v>30</v>
       </c>
+      <c r="G13" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="str">
@@ -820,6 +863,9 @@
       <c r="F14" t="s">
         <v>29</v>
       </c>
+      <c r="G14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="str">
@@ -841,6 +887,9 @@
       <c r="F15" t="s">
         <v>30</v>
       </c>
+      <c r="G15" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="str">
@@ -862,8 +911,11 @@
       <c r="F16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="str">
         <f t="shared" si="0"/>
         <v>2.6.1</v>
@@ -883,8 +935,11 @@
       <c r="F17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="str">
         <f t="shared" si="0"/>
         <v>3.1.1</v>
@@ -904,8 +959,11 @@
       <c r="F18" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="str">
         <f t="shared" si="0"/>
         <v>3.1.2</v>
@@ -925,8 +983,11 @@
       <c r="F19" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="str">
         <f t="shared" si="0"/>
         <v>3.2.1</v>
@@ -946,8 +1007,11 @@
       <c r="F20" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="str">
         <f t="shared" si="0"/>
         <v>3.2.2</v>
@@ -967,8 +1031,11 @@
       <c r="F21" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="str">
         <f t="shared" si="0"/>
         <v>3.3.1</v>
@@ -988,8 +1055,11 @@
       <c r="F22" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="str">
         <f t="shared" si="0"/>
         <v>3.3.2</v>
@@ -1009,8 +1079,11 @@
       <c r="F23" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="str">
         <f t="shared" si="0"/>
         <v>3.4.1</v>
@@ -1030,8 +1103,11 @@
       <c r="F24" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="str">
         <f t="shared" si="0"/>
         <v>3.4.2</v>
@@ -1051,8 +1127,11 @@
       <c r="F25" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="str">
         <f t="shared" si="0"/>
         <v>3.5.1</v>
@@ -1071,6 +1150,9 @@
       </c>
       <c r="F26" t="s">
         <v>34</v>
+      </c>
+      <c r="G26" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>